<commit_message>
Finished export to Excel capability. Added integration tests and spreadsheet for integration testing.
</commit_message>
<xml_diff>
--- a/IPGMMSIntegrationTests/IntegrationTestPanel.xlsx
+++ b/IPGMMSIntegrationTests/IntegrationTestPanel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -42,6 +42,33 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Alvarado</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Member should be found when searched for</t>
+  </si>
+  <si>
+    <t>Member update page should show information for the correct member</t>
+  </si>
+  <si>
+    <t>Basic member information can be updated.</t>
+  </si>
+  <si>
+    <t>Error occurs if user tries to enter data other than a date into 'Update Member Info' page</t>
+  </si>
+  <si>
+    <t>Member mailing information can be updated.</t>
+  </si>
+  <si>
+    <t>Member listing information can be updated.</t>
+  </si>
+  <si>
+    <t>Multiple mailing information fields can be updated at once</t>
   </si>
 </sst>
 </file>
@@ -49,7 +76,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -66,12 +93,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -129,28 +162,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -468,60 +502,130 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="5"/>
+    <row r="2" spans="1:6" ht="35.4" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="5">
+        <v>64</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="7">
+        <v>42866</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" s="8"/>
-      <c r="B3" s="9"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
+    <row r="3" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A3" s="8">
+        <v>64</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="7">
+        <v>42866</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="8"/>
-      <c r="B4" s="9"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8"/>
+    <row r="4" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A4" s="8">
+        <v>64</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7">
+        <v>42866</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="8"/>
+    <row r="5" spans="1:6" ht="69.599999999999994" x14ac:dyDescent="0.4">
+      <c r="A5" s="8">
+        <v>64</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7">
+        <v>42866</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="8"/>
+    <row r="6" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A6" s="8">
+        <v>64</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="7">
+        <v>42866</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F6" s="9"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" s="8"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="8"/>
+    <row r="7" spans="1:6" ht="34.799999999999997" x14ac:dyDescent="0.4">
+      <c r="A7" s="8">
+        <v>64</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="7">
+        <v>42866</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" s="8"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="8"/>
+    <row r="8" spans="1:6" ht="52.2" x14ac:dyDescent="0.4">
+      <c r="A8" s="8">
+        <v>64</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="7">
+        <v>42866</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>7</v>
+      </c>
       <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.4">

</xml_diff>